<commit_message>
add level selector for talent
</commit_message>
<xml_diff>
--- a/data/attack_talents.xlsx
+++ b/data/attack_talents.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nonext\PycharmProjects\GenshinAutoInfo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C234C560-3756-4DFA-93B5-6E930DE37330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344E1086-8118-491C-9252-1F2C49E76604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="1545" windowWidth="21705" windowHeight="13080" tabRatio="731" firstSheet="37" activeTab="39" xr2:uid="{814E84DE-4A35-430B-95F4-3ACD911E6434}"/>
+    <workbookView xWindow="1185" yWindow="330" windowWidth="15600" windowHeight="14475" tabRatio="731" activeTab="2" xr2:uid="{814E84DE-4A35-430B-95F4-3ACD911E6434}"/>
   </bookViews>
   <sheets>
     <sheet name="Amber" sheetId="1" r:id="rId1"/>
-    <sheet name="Barbaara" sheetId="2" r:id="rId2"/>
+    <sheet name="Barbara" sheetId="2" r:id="rId2"/>
     <sheet name="Beidou" sheetId="3" r:id="rId3"/>
     <sheet name="Bennett" sheetId="4" r:id="rId4"/>
     <sheet name="Chongyun" sheetId="5" r:id="rId5"/>
@@ -17891,7 +17891,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>21</v>
@@ -18044,7 +18044,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
         <v>24</v>
@@ -18299,7 +18299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>30</v>
@@ -18350,7 +18350,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>31</v>
@@ -18475,7 +18475,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -18526,7 +18526,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -18577,7 +18577,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -18679,7 +18679,7 @@
         <v>2173</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="19" t="s">
         <v>81</v>
@@ -18730,7 +18730,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>19</v>
@@ -18832,7 +18832,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="19" t="s">
         <v>83</v>
@@ -18883,7 +18883,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="14" t="s">
         <v>22</v>
@@ -18985,7 +18985,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="21" t="s">
         <v>24</v>
@@ -19088,7 +19088,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>84</v>
@@ -19139,7 +19139,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>62</v>
@@ -19190,7 +19190,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>375</v>
@@ -19292,7 +19292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>43</v>
@@ -19343,7 +19343,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>86</v>
@@ -19394,7 +19394,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="14" t="s">
         <v>102</v>
@@ -19517,7 +19517,7 @@
       <c r="S1" s="14"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -19569,7 +19569,7 @@
       </c>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -19621,7 +19621,7 @@
       </c>
       <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -19673,7 +19673,7 @@
       </c>
       <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>33</v>
@@ -19829,7 +19829,7 @@
       </c>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="21" t="s">
         <v>24</v>
@@ -19985,7 +19985,7 @@
       </c>
       <c r="R10" s="14"/>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="14" t="s">
         <v>4853</v>
@@ -20088,7 +20088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>4855</v>
@@ -20228,7 +20228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -20279,7 +20279,7 @@
         <v>2279</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -20330,7 +20330,7 @@
         <v>2293</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -20381,7 +20381,7 @@
         <v>2308</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -20432,7 +20432,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>33</v>
@@ -20483,7 +20483,7 @@
         <v>2337</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>22</v>
@@ -20585,7 +20585,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="17" t="s">
         <v>24</v>
@@ -20687,7 +20687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="14" t="s">
         <v>50</v>
@@ -20738,7 +20738,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>107</v>
@@ -20789,7 +20789,7 @@
         <v>2362</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>108</v>
@@ -20840,7 +20840,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>109</v>
@@ -20891,7 +20891,7 @@
         <v>2389</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>110</v>
@@ -20994,7 +20994,7 @@
       </c>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>112</v>
@@ -21115,7 +21115,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -21166,7 +21166,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -21217,7 +21217,7 @@
         <v>2446</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -21268,7 +21268,7 @@
         <v>2459</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -21319,7 +21319,7 @@
         <v>2472</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>33</v>
@@ -21370,7 +21370,7 @@
         <v>2487</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>22</v>
@@ -21472,7 +21472,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="17" t="s">
         <v>24</v>
@@ -21626,7 +21626,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>28</v>
@@ -21729,7 +21729,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>116</v>
@@ -21850,7 +21850,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>118</v>
@@ -21901,7 +21901,7 @@
         <v>2544</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>33</v>
@@ -21952,7 +21952,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>119</v>
@@ -22003,7 +22003,7 @@
         <v>2573</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="30" t="s">
         <v>22</v>
@@ -22105,7 +22105,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="31" t="s">
         <v>24</v>
@@ -22208,7 +22208,7 @@
       </c>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="6" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="14" t="s">
         <v>27</v>
@@ -22362,7 +22362,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>122</v>
@@ -22483,7 +22483,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -22534,7 +22534,7 @@
         <v>2611</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -22585,7 +22585,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -22636,7 +22636,7 @@
         <v>2638</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -22687,7 +22687,7 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>37</v>
@@ -22738,7 +22738,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>38</v>
@@ -22789,7 +22789,7 @@
         <v>2680</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -22891,7 +22891,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -22993,7 +22993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -23095,7 +23095,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>392</v>
@@ -23198,7 +23198,7 @@
       </c>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>126</v>
@@ -23249,7 +23249,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>43</v>
@@ -23300,7 +23300,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>393</v>
@@ -23440,7 +23440,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -23491,7 +23491,7 @@
         <v>2714</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -23644,7 +23644,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -23746,7 +23746,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -23848,7 +23848,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -23951,7 +23951,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -24104,7 +24104,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>131</v>
@@ -24206,7 +24206,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>43</v>
@@ -24257,7 +24257,7 @@
         <v>2761</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>392</v>
@@ -24396,7 +24396,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -24447,7 +24447,7 @@
         <v>2773</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -24498,7 +24498,7 @@
         <v>2788</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -24549,7 +24549,7 @@
         <v>2803</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -24600,7 +24600,7 @@
         <v>2817</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>37</v>
@@ -24651,7 +24651,7 @@
         <v>2829</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>38</v>
@@ -24702,7 +24702,7 @@
         <v>2841</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -24804,7 +24804,7 @@
         <v>2868</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -24906,7 +24906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>135</v>
@@ -24957,7 +24957,7 @@
         <v>2895</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>136</v>
@@ -25059,7 +25059,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>73</v>
@@ -25110,7 +25110,7 @@
         <v>2922</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>138</v>
@@ -25231,7 +25231,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -25282,7 +25282,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -25333,7 +25333,7 @@
         <v>2952</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -25384,7 +25384,7 @@
         <v>2967</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -25435,7 +25435,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>33</v>
@@ -25486,7 +25486,7 @@
         <v>2993</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>22</v>
@@ -25588,7 +25588,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="17" t="s">
         <v>24</v>
@@ -25690,7 +25690,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="14" t="s">
         <v>43</v>
@@ -25843,7 +25843,7 @@
         <v>3021</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>142</v>
@@ -25964,7 +25964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -26015,7 +26015,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -26066,7 +26066,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -26117,7 +26117,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -26168,7 +26168,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -26270,7 +26270,7 @@
         <v>4849</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -26372,7 +26372,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -26475,7 +26475,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>145</v>
@@ -26526,7 +26526,7 @@
         <v>3042</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>146</v>
@@ -26577,7 +26577,7 @@
         <v>3056</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>147</v>
@@ -26628,7 +26628,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>148</v>
@@ -26730,7 +26730,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>150</v>
@@ -26781,7 +26781,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>142</v>
@@ -26904,7 +26904,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -26955,7 +26955,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -27006,7 +27006,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -27057,7 +27057,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -27108,7 +27108,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="14" t="s">
         <v>33</v>
@@ -27159,7 +27159,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="14" t="s">
         <v>22</v>
@@ -27465,7 +27465,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="14" t="s">
         <v>35</v>
@@ -27567,7 +27567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="14" t="s">
         <v>371</v>
@@ -27689,7 +27689,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -27740,7 +27740,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -27791,7 +27791,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -27842,7 +27842,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -27893,7 +27893,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -27995,7 +27995,7 @@
         <v>4834</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -28097,7 +28097,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -28199,7 +28199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>145</v>
@@ -28250,7 +28250,7 @@
         <v>3042</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>146</v>
@@ -28301,7 +28301,7 @@
         <v>3056</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>147</v>
@@ -28352,7 +28352,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>148</v>
@@ -28454,7 +28454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>150</v>
@@ -28505,7 +28505,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>142</v>
@@ -28681,7 +28681,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -28732,7 +28732,7 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -28834,7 +28834,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -28885,7 +28885,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>152</v>
@@ -28936,7 +28936,7 @@
         <v>3156</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>20</v>
@@ -28987,7 +28987,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="14" t="s">
         <v>21</v>
@@ -29038,7 +29038,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="14" t="s">
         <v>22</v>
@@ -29140,7 +29140,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="21" t="s">
         <v>24</v>
@@ -29243,7 +29243,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>50</v>
@@ -29294,7 +29294,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>154</v>
@@ -29448,7 +29448,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>142</v>
@@ -29569,7 +29569,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -29620,7 +29620,7 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -29722,7 +29722,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -29773,7 +29773,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -29824,7 +29824,7 @@
         <v>3251</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>33</v>
@@ -29875,7 +29875,7 @@
         <v>3265</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -29977,7 +29977,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="24" t="s">
         <v>24</v>
@@ -30080,7 +30080,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>173</v>
@@ -30183,7 +30183,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>175</v>
@@ -30234,7 +30234,7 @@
         <v>3289</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>176</v>
@@ -30285,7 +30285,7 @@
         <v>3293</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>177</v>
@@ -30336,7 +30336,7 @@
         <v>3308</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>178</v>
@@ -30576,7 +30576,7 @@
         <v>3331</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -30729,7 +30729,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>152</v>
@@ -30780,7 +30780,7 @@
         <v>3374</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>33</v>
@@ -30831,7 +30831,7 @@
         <v>3388</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>22</v>
@@ -30933,7 +30933,7 @@
         <v>3417</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="21" t="s">
         <v>24</v>
@@ -31036,7 +31036,7 @@
       </c>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>43</v>
@@ -31138,7 +31138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>182</v>
@@ -31261,7 +31261,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -31312,7 +31312,7 @@
         <v>3499</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -31414,7 +31414,7 @@
         <v>3485</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -31618,7 +31618,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>22</v>
@@ -31720,7 +31720,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="21" t="s">
         <v>24</v>
@@ -31925,7 +31925,7 @@
       </c>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>186</v>
@@ -32067,7 +32067,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -32118,7 +32118,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -32169,7 +32169,7 @@
         <v>3593</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -32220,7 +32220,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -32271,7 +32271,7 @@
         <v>3618</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20" t="s">
         <v>19</v>
@@ -32322,7 +32322,7 @@
         <v>3631</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="20" t="s">
         <v>152</v>
@@ -32373,7 +32373,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>20</v>
@@ -32424,7 +32424,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>21</v>
@@ -32475,7 +32475,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="20" t="s">
         <v>188</v>
@@ -32526,7 +32526,7 @@
         <v>3555</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="20" t="s">
         <v>189</v>
@@ -32577,7 +32577,7 @@
         <v>3656</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="20" t="s">
         <v>22</v>
@@ -32679,7 +32679,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="21" t="s">
         <v>24</v>
@@ -32833,7 +32833,7 @@
         <v>3289</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>15</v>
@@ -32884,7 +32884,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>16</v>
@@ -32935,7 +32935,7 @@
         <v>3669</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>17</v>
@@ -32986,7 +32986,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="14" t="s">
         <v>18</v>
@@ -33037,7 +33037,7 @@
         <v>3692</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="14" t="s">
         <v>19</v>
@@ -33537,7 +33537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -33588,7 +33588,7 @@
         <v>3798</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -33639,7 +33639,7 @@
         <v>3812</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -33690,7 +33690,7 @@
         <v>3826</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -33741,7 +33741,7 @@
         <v>3837</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -33792,7 +33792,7 @@
         <v>3770</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>152</v>
@@ -33843,7 +33843,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>33</v>
@@ -33894,7 +33894,7 @@
         <v>3865</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="23" t="s">
         <v>22</v>
@@ -33996,7 +33996,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="24" t="s">
         <v>24</v>
@@ -34150,7 +34150,7 @@
         <v>3878</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="19" t="s">
         <v>202</v>
@@ -34201,7 +34201,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>154</v>
@@ -34252,7 +34252,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>199</v>
@@ -34303,7 +34303,7 @@
         <v>3898</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>200</v>
@@ -34406,7 +34406,7 @@
       </c>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>43</v>
@@ -34546,7 +34546,7 @@
       </c>
       <c r="R1" s="11"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="23" t="s">
         <v>15</v>
@@ -34597,7 +34597,7 @@
         <v>3949</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="23" t="s">
         <v>16</v>
@@ -34648,7 +34648,7 @@
         <v>3614</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="23" t="s">
         <v>17</v>
@@ -34699,7 +34699,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="23" t="s">
         <v>18</v>
@@ -34750,7 +34750,7 @@
         <v>2059</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="23" t="s">
         <v>19</v>
@@ -34801,7 +34801,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="23" t="s">
         <v>20</v>
@@ -34852,7 +34852,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="23" t="s">
         <v>21</v>
@@ -34903,7 +34903,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="23" t="s">
         <v>22</v>
@@ -35005,7 +35005,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="24" t="s">
         <v>24</v>
@@ -35261,7 +35261,7 @@
       </c>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>43</v>
@@ -35312,7 +35312,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>224</v>
@@ -35504,7 +35504,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -35555,7 +35555,7 @@
         <v>4038</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -35606,7 +35606,7 @@
         <v>4051</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -35657,7 +35657,7 @@
         <v>4062</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -35708,7 +35708,7 @@
         <v>4077</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20" t="s">
         <v>37</v>
@@ -35759,7 +35759,7 @@
         <v>4090</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="20" t="s">
         <v>38</v>
@@ -35810,7 +35810,7 @@
         <v>2841</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>22</v>
@@ -35912,7 +35912,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="21" t="s">
         <v>24</v>
@@ -36320,7 +36320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>43</v>
@@ -36371,7 +36371,7 @@
         <v>4123</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>233</v>
@@ -36519,7 +36519,7 @@
       </c>
       <c r="R1" s="11"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="23" t="s">
         <v>15</v>
@@ -36570,7 +36570,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="23" t="s">
         <v>16</v>
@@ -36621,7 +36621,7 @@
         <v>4148</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="23" t="s">
         <v>17</v>
@@ -36672,7 +36672,7 @@
         <v>4160</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="23" t="s">
         <v>18</v>
@@ -36723,7 +36723,7 @@
         <v>4160</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="23" t="s">
         <v>19</v>
@@ -36774,7 +36774,7 @@
         <v>4174</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="23" t="s">
         <v>152</v>
@@ -36825,7 +36825,7 @@
         <v>4188</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="23" t="s">
         <v>20</v>
@@ -36876,7 +36876,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="23" t="s">
         <v>235</v>
@@ -36927,7 +36927,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="23" t="s">
         <v>236</v>
@@ -36978,7 +36978,7 @@
         <v>2919</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="23" t="s">
         <v>237</v>
@@ -37029,7 +37029,7 @@
         <v>4197</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="23" t="s">
         <v>22</v>
@@ -37131,7 +37131,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="24" t="s">
         <v>24</v>
@@ -37233,7 +37233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>27</v>
@@ -37284,7 +37284,7 @@
         <v>3755</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>43</v>
@@ -37387,7 +37387,7 @@
       </c>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>240</v>
@@ -37465,7 +37465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B263D45-7313-4E89-BA83-CCAB0EB22738}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -37526,7 +37526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -37577,7 +37577,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -37628,7 +37628,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -37679,7 +37679,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -37730,7 +37730,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -37781,7 +37781,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>37</v>
@@ -37832,7 +37832,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>38</v>
@@ -37883,7 +37883,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="14" t="s">
         <v>22</v>
@@ -37985,7 +37985,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
         <v>24</v>
@@ -38088,7 +38088,7 @@
       </c>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>372</v>
@@ -38140,7 +38140,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>40</v>
@@ -38294,7 +38294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>43</v>
@@ -38345,7 +38345,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>44</v>
@@ -38396,7 +38396,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>45</v>
@@ -38518,7 +38518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="23" t="s">
         <v>15</v>
@@ -38569,7 +38569,7 @@
         <v>4242</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="23" t="s">
         <v>16</v>
@@ -38620,7 +38620,7 @@
         <v>4242</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="23" t="s">
         <v>17</v>
@@ -38671,7 +38671,7 @@
         <v>4257</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="23" t="s">
         <v>18</v>
@@ -38875,7 +38875,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="23" t="s">
         <v>22</v>
@@ -38977,7 +38977,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="24" t="s">
         <v>24</v>
@@ -39079,7 +39079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>43</v>
@@ -39130,7 +39130,7 @@
         <v>4295</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>243</v>
@@ -39233,7 +39233,7 @@
       </c>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>73</v>
@@ -39284,7 +39284,7 @@
         <v>4309</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>245</v>
@@ -39428,7 +39428,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -39479,7 +39479,7 @@
         <v>4352</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -39530,7 +39530,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -39734,7 +39734,7 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>104</v>
@@ -39785,7 +39785,7 @@
         <v>4382</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>22</v>
@@ -39887,7 +39887,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="21" t="s">
         <v>24</v>
@@ -39990,7 +39990,7 @@
       </c>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>43</v>
@@ -40284,7 +40284,7 @@
       </c>
       <c r="R1" s="18"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -40335,7 +40335,7 @@
         <v>4425</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -40386,7 +40386,7 @@
         <v>4440</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -40437,7 +40437,7 @@
         <v>4452</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -40488,7 +40488,7 @@
         <v>4397</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20" t="s">
         <v>19</v>
@@ -40539,7 +40539,7 @@
         <v>4464</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="20" t="s">
         <v>33</v>
@@ -40590,7 +40590,7 @@
         <v>4412</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>104</v>
@@ -40641,7 +40641,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>22</v>
@@ -40743,7 +40743,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="21" t="s">
         <v>24</v>
@@ -40846,7 +40846,7 @@
       </c>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>43</v>
@@ -40949,7 +40949,7 @@
       </c>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>253</v>
@@ -41000,7 +41000,7 @@
         <v>4493</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>254</v>
@@ -41140,7 +41140,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -41191,7 +41191,7 @@
         <v>4561</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -41242,7 +41242,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -41446,7 +41446,7 @@
         <v>4609</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>256</v>
@@ -41497,7 +41497,7 @@
         <v>4622</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>22</v>
@@ -41599,7 +41599,7 @@
         <v>4640</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="21" t="s">
         <v>24</v>
@@ -41702,7 +41702,7 @@
       </c>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>258</v>
@@ -41753,7 +41753,7 @@
         <v>4520</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>259</v>
@@ -41855,7 +41855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>43</v>
@@ -41906,7 +41906,7 @@
         <v>4671</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>261</v>
@@ -41957,7 +41957,7 @@
         <v>4686</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>262</v>
@@ -42008,7 +42008,7 @@
         <v>4534</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>263</v>
@@ -42148,7 +42148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -42199,7 +42199,7 @@
         <v>4975</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -42250,7 +42250,7 @@
         <v>4987</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -42454,7 +42454,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="21" t="s">
         <v>24</v>
@@ -42556,7 +42556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="14" t="s">
         <v>43</v>
@@ -42659,7 +42659,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -42710,7 +42710,7 @@
         <v>5011</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>267</v>
@@ -42851,7 +42851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="23" t="s">
         <v>15</v>
@@ -42902,7 +42902,7 @@
         <v>5063</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="23" t="s">
         <v>16</v>
@@ -43004,7 +43004,7 @@
         <v>5034</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="23" t="s">
         <v>18</v>
@@ -43106,7 +43106,7 @@
         <v>5049</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="23" t="s">
         <v>37</v>
@@ -43157,7 +43157,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="23" t="s">
         <v>38</v>
@@ -43208,7 +43208,7 @@
         <v>5104</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="23" t="s">
         <v>22</v>
@@ -43310,7 +43310,7 @@
         <v>5114</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="24" t="s">
         <v>24</v>
@@ -43413,7 +43413,7 @@
       </c>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>50</v>
@@ -43464,7 +43464,7 @@
         <v>5132</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>154</v>
@@ -43515,7 +43515,7 @@
         <v>5147</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>270</v>
@@ -43617,7 +43617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>43</v>
@@ -43668,7 +43668,7 @@
         <v>5147</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>272</v>
@@ -43719,7 +43719,7 @@
         <v>5162</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="14" t="s">
         <v>273</v>
@@ -43867,7 +43867,7 @@
       </c>
       <c r="R1" s="11"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="23" t="s">
         <v>15</v>
@@ -43918,7 +43918,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="23" t="s">
         <v>16</v>
@@ -43969,7 +43969,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="23" t="s">
         <v>17</v>
@@ -44020,7 +44020,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="23" t="s">
         <v>18</v>
@@ -44071,7 +44071,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="23" t="s">
         <v>19</v>
@@ -44173,7 +44173,7 @@
         <v>5184</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="23" t="s">
         <v>22</v>
@@ -44275,7 +44275,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="24" t="s">
         <v>24</v>
@@ -44378,7 +44378,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -44481,7 +44481,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>277</v>
@@ -44628,7 +44628,7 @@
       </c>
       <c r="Q1" s="18"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -44679,7 +44679,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -44730,7 +44730,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -44781,7 +44781,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -44832,7 +44832,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20" t="s">
         <v>19</v>
@@ -45036,7 +45036,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="21" t="s">
         <v>24</v>
@@ -45138,7 +45138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -45240,7 +45240,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>277</v>
@@ -45378,7 +45378,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -45429,7 +45429,7 @@
         <v>5267</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -45531,7 +45531,7 @@
         <v>5223</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -45582,7 +45582,7 @@
         <v>5285</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -45684,7 +45684,7 @@
         <v>5253</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -45786,7 +45786,7 @@
         <v>3417</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -45888,7 +45888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>135</v>
@@ -45939,7 +45939,7 @@
         <v>3076</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>136</v>
@@ -46041,7 +46041,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>62</v>
@@ -46143,7 +46143,7 @@
         <v>3755</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>142</v>
@@ -46282,7 +46282,7 @@
       </c>
       <c r="R1" s="18"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -46333,7 +46333,7 @@
         <v>5357</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -46384,7 +46384,7 @@
         <v>5368</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -46435,7 +46435,7 @@
         <v>5381</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -46486,7 +46486,7 @@
         <v>5327</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20" t="s">
         <v>19</v>
@@ -46537,7 +46537,7 @@
         <v>5394</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="20" t="s">
         <v>20</v>
@@ -46588,7 +46588,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>21</v>
@@ -46639,7 +46639,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>282</v>
@@ -46690,7 +46690,7 @@
         <v>5407</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="20" t="s">
         <v>22</v>
@@ -46792,7 +46792,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="21" t="s">
         <v>24</v>
@@ -46996,7 +46996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>43</v>
@@ -47047,7 +47047,7 @@
         <v>5414</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
         <v>286</v>
@@ -47186,7 +47186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -47237,7 +47237,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -47288,7 +47288,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -47339,7 +47339,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -47390,7 +47390,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -47492,7 +47492,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="19" t="s">
         <v>47</v>
@@ -47543,7 +47543,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="14" t="s">
         <v>22</v>
@@ -47645,7 +47645,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
         <v>24</v>
@@ -47747,7 +47747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>50</v>
@@ -47849,7 +47849,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="19" t="s">
         <v>51</v>
@@ -47951,7 +47951,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="19" t="s">
         <v>54</v>
@@ -48002,7 +48002,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>28</v>
@@ -48105,7 +48105,7 @@
       </c>
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="14" t="s">
         <v>43</v>
@@ -48234,7 +48234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD47BC6C-7C97-4DDD-9EDE-012FDD36AC65}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -48298,7 +48298,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -48349,7 +48349,7 @@
         <v>5478</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -48451,7 +48451,7 @@
         <v>5438</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -48502,7 +48502,7 @@
         <v>5506</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20" t="s">
         <v>37</v>
@@ -48553,7 +48553,7 @@
         <v>5510</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="20" t="s">
         <v>38</v>
@@ -48604,7 +48604,7 @@
         <v>5515</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>22</v>
@@ -48706,7 +48706,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="21" t="s">
         <v>24</v>
@@ -48809,7 +48809,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>289</v>
@@ -48860,7 +48860,7 @@
         <v>2446</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>290</v>
@@ -48911,7 +48911,7 @@
         <v>5524</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>291</v>
@@ -48962,7 +48962,7 @@
         <v>4197</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>292</v>
@@ -49013,7 +49013,7 @@
         <v>3056</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>293</v>
@@ -49115,7 +49115,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>295</v>
@@ -49217,7 +49217,7 @@
         <v>5453</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="14" t="s">
         <v>297</v>
@@ -49411,7 +49411,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -49462,7 +49462,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="20" t="s">
         <v>16</v>
@@ -49513,7 +49513,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="20" t="s">
         <v>17</v>
@@ -49564,7 +49564,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
@@ -49615,7 +49615,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20" t="s">
         <v>19</v>
@@ -49717,7 +49717,7 @@
         <v>5184</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>22</v>
@@ -49819,7 +49819,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="21" t="s">
         <v>24</v>
@@ -49921,7 +49921,7 @@
       </c>
       <c r="Q11" s="18"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -50024,7 +50024,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>43</v>
@@ -50075,7 +50075,7 @@
         <v>5577</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>69</v>
@@ -50217,7 +50217,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="23" t="s">
         <v>15</v>
@@ -50268,7 +50268,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="23" t="s">
         <v>16</v>
@@ -50319,7 +50319,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="23" t="s">
         <v>17</v>
@@ -50370,7 +50370,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="23" t="s">
         <v>18</v>
@@ -50421,7 +50421,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="23" t="s">
         <v>19</v>
@@ -50523,7 +50523,7 @@
         <v>5208</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="23" t="s">
         <v>22</v>
@@ -50625,7 +50625,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="24" t="s">
         <v>24</v>
@@ -50727,7 +50727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -50829,7 +50829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>43</v>
@@ -50880,7 +50880,7 @@
         <v>5577</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>69</v>
@@ -51723,7 +51723,7 @@
       </c>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>316</v>
       </c>
@@ -51932,7 +51932,7 @@
         <v>5655</v>
       </c>
     </row>
-    <row r="20" spans="2:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>348</v>
       </c>
@@ -54365,7 +54365,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -54416,7 +54416,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -54467,7 +54467,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -54518,7 +54518,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -54569,7 +54569,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>37</v>
@@ -54620,7 +54620,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>38</v>
@@ -54671,7 +54671,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -54773,7 +54773,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -54876,7 +54876,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -54979,7 +54979,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>43</v>
@@ -55100,7 +55100,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -55151,7 +55151,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -55202,7 +55202,7 @@
         <v>1614</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -55253,7 +55253,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -55304,7 +55304,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>37</v>
@@ -55355,7 +55355,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>38</v>
@@ -55406,7 +55406,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -55508,7 +55508,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -55610,7 +55610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>15</v>
@@ -55661,7 +55661,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>16</v>
@@ -55712,7 +55712,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>17</v>
@@ -55815,7 +55815,7 @@
       </c>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>62</v>
@@ -55917,7 +55917,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="14" t="s">
         <v>28</v>
@@ -56040,7 +56040,7 @@
       </c>
       <c r="Q1" s="18"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -56091,7 +56091,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -56142,7 +56142,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -56193,7 +56193,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -56244,7 +56244,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -56295,7 +56295,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>20</v>
@@ -56346,7 +56346,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>21</v>
@@ -56397,7 +56397,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="14" t="s">
         <v>22</v>
@@ -56499,7 +56499,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
         <v>24</v>
@@ -56601,7 +56601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>66</v>
@@ -56652,7 +56652,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>67</v>
@@ -56755,7 +56755,7 @@
       </c>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
         <v>69</v>
@@ -56877,7 +56877,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -56928,7 +56928,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -56979,7 +56979,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -57030,7 +57030,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -57081,7 +57081,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -57132,7 +57132,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>33</v>
@@ -57183,7 +57183,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="14" t="s">
         <v>22</v>
@@ -57285,7 +57285,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
         <v>24</v>
@@ -57388,7 +57388,7 @@
       </c>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -57491,7 +57491,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>73</v>
@@ -57542,7 +57542,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>74</v>
@@ -57784,7 +57784,7 @@
       </c>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -57835,7 +57835,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -57886,7 +57886,7 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -57937,7 +57937,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>18</v>
@@ -57988,7 +57988,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>19</v>
@@ -58090,7 +58090,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="19" t="s">
         <v>47</v>
@@ -58141,7 +58141,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="14" t="s">
         <v>22</v>
@@ -58243,7 +58243,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
         <v>24</v>
@@ -58345,7 +58345,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="14" t="s">
         <v>43</v>
@@ -58448,7 +58448,7 @@
       </c>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
         <v>43</v>

</xml_diff>